<commit_message>
fix: correct mis-pasted data
</commit_message>
<xml_diff>
--- a/LWCF/Data/StateGrantData/GA_LWCFGrants1965-2011.xlsx
+++ b/LWCF/Data/StateGrantData/GA_LWCFGrants1965-2011.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherkusmierz/GitHub/DataScienceforConservation/LWCF/Data/StateGrantData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7107AA-E6F8-5E49-A4D6-1E30F7A78C27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD2198A-4363-7043-A9E1-8E91A8EFC26C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{B6F33490-F3E6-7A4C-BEE8-2FF3B7EA137C}"/>
   </bookViews>
   <sheets>
     <sheet name="GA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4012" uniqueCount="1669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4017" uniqueCount="1669">
   <si>
     <t>Grant ID &amp; Element</t>
   </si>
@@ -3915,341 +3915,6 @@
     <t>CITY OF WALNUT GROVE</t>
   </si>
   <si>
-    <t xml:space="preserve">BILL MORRIS PARK	CITY OF JESUP &amp; WAYNE COUNTY	WAYNE	GA	$20,200.00	1977	1979	Acquisition
-377 - XXX	WHITE COUNTY PARK	WHITE COUNTY	WHITE	GA	$45,630.46	1977	1982	Development
-446 - XXX	ALMA-BACON RECREATION PARK 1978	CITY OF ALMA &amp; BACON COUNTY	BACON	GA	$10,100.00	1978	1980	Development
-420 - XXX	ATCO PARK	CITY OF CARTERSVILLE	BARTOW	GA	$15,261.45	1978	1981	Development
-444 - XXX	CASSVILLE PARK	BARTOW COUNTY	BARTOW	GA	$41,239.95	1978	1980	Development
-442 - XXX	FARMER'S MARKET PARK	CITY OF NASHVILLE	BERRIEN	GA	$17,105.26	1978	1980	Development
-454 - XXX	NORTHSIDE PARK	CITY OF MACON	BIBB	GA	$222,200.00	1978	1980	Development
-473 - XXX	COCHRAN/BLECKLEY COUNTY RECREATION A	CITY OF COCHRAN &amp; BLECKLEY COUNTY	BLECKLEY	GA	$37,441.56	1978	1983	Combination
-431 - XXX	GEORGE A. ROEBUCK REC. COMPLEX	CITY OF BROOKLET	BULLOCH	GA	$8,828.38	1978	1982	Development
-439 - XXX	ARLINGTON PARK	CITY OF ARLINGTON	CALHOUN	GA	$10,100.00	1978	1980	Development
-453 - XXX	BOWDON RECREATION PARK	CITY OF BOWDON	CARROLL	GA	$30,300.00	1978	1980	Development
-427 - XXX	SAVANNAH PARK'S DEVELOPMENT 1978	CITY OF SAVANNAH	CHATHAM	GA	$56,113.47	1978	1980	Development
-461 - XXX	TYBEE ISLAND PARK	CITY OF TYBEE ISLAND	CHATHAM	GA	$58,609.68	1978	1981	Development
-424 - XXX	BISHOP PARK	CITY OF ATHENS	CLARKE	GA	$15,150.00	1978	1980	Development
-421 - XXX	FORT GAINES CITY PARK	CITY OF FORT GAINES	CLAY	GA	$13,130.00	1978	1980	Development
-437 - XXX	COLLEGE PARK DEVELOPMENTS, 1978	CITY OF COLLEGE PARK	CLAYTON	GA	$20,800.76	1978	1980	Development
-430 - XXX	HURT ROAD PARK	COBB COUNTY	COBB	GA	$204,131.28	1978	1983	Development
-447 - XXX	LEWIS PARK	CITY OF MARIETTA	COBB	GA	$22,725.00	1978	1980	Development
-433 - XXX	LITHONIA COMMUNITY PARK	DEKALB COUNTY	DEKALB	GA	$150,826.04	1978	1983	Combination
-434 - XXX	REDAN PARK	DEKALB COUNTY	DEKALB	GA	$163,750.88	1978	1980	Combination
-457 - XXX	CEDAR PARK	DEKALB COUNTY	DEKALB	GA	$120,986.23	1978	1980	Development
-458 - XXX	BRUCE STREET PARK	DEKALB COUNTY	DEKALB	GA	$19,959.60	1978	1980	Development
-445 - XXX	CHEHAW PARK	CITY OF ALBANY	DOUGHERTY	GA	$6,628.76	1978	1980	Development
-438 - XXX	EVANS COUNTY PARK-PHASE I	EVANS COUNTY	EVANS	GA	$133,979.48	1978	1982	Development
-440 - XXX	BLUERIDGE CITY PARK PHASE II	CITY OF BLUE RIDGE	FANNIN	GA	$12,514.23	1978	1980	Development
-417 - XXX	KIWANIS PARK	FAYETTE COUNTY	FAYETTE	GA	$9,962.82	1978	1980	Development
-449 - XXX	RILEY FIELD, PEACHTREE CITY	CITY OF PEACHTREE CITY	FAYETTE	GA	$44,793.37	1978	1981	Combination
-425 - XXX	CUMMING CITY PARK II	CITY OF CUMMING	FORSYTH	GA	$30,300.00	1978	1980	Development
-435 - XXX	ROSWELL AREA PARK	CITY OF ROSWELL	FULTON	GA	$30,253.14	1978	1980	Development
-459 - XXX	ATLANTA PARK IMPROVEMENTS 1978	CITY OF ATLANTA	FULTON	GA	$547,332.00	1978	1982	Development
-467 - XXX	BEST FRIEND &amp; SHORTY HOWELL PARKS	GWINNETT COUNTY	GWINNETT	GA	$42,161.83	1978	1983	Development
-426 - XXX	CORNELIA PARKS DEVELOPMENT	CITY OF CORNELIA	HABERSHAM	GA	$29,557.79	1978	1983	Development
-450 - XXX	HALL COUNTY CENTRAL PARK	HALL COUNTY	HALL	GA	$125,210.95	1978	1981	Combination
-474 - XXX	BUCHANAN CITY PARK	CITY OF BUCHANAN	HARALSON	GA	$75,750.00	1978	1983	Acquisition
-422 - XXX	PINEMOUNTAIN CITY PARK II	CITY OF PINE MOUNTAIN	HARRIS	GA	$7,794.57	1978	1981	Development
-428 - XXX	JESSE TANNER MEMORIAL PARK	CITY OF WARNER ROBINS	HOUSTON	GA	$40,400.00	1978	1980	Development
-416 - XXX	COMMERCE ATHLETIC PARK	CITY OF COMMERCE	JACKSON	GA	$38,234.99	1978	1983	Development
-448 - XXX	RABUN PARK	CITY OF WRENS	JEFFERSON	GA	$25,250.00	1978	1980	Development
-469 - XXX	BARNESVILLE-LAMAR COUNTY PARK EAST	CITY OF BARNESVILLE-LAMAR COUNTY	LAMAR	GA	$30,300.00	1978	1980	Development
-456 - XXX	SPRINGDALE PARK	CITY OF DUBLIN	LAURENS	GA	$83,973.06	1978	1984	Combination
-470 - XXX	SWEETWATER PARK	CITY OF THOMSON &amp; MCDUFFIE CO.	MCDUFFIE	GA	$50,877.03	1978	1983	Combination
-443 - XXX	COLUMBUS NEIGHBORHOOD PARKS	CITY OF COLUMBUS	MUSCOGEE	GA	$111,100.00	1978	1980	Development
-441 - XXX	CUTHBERT CITY PARK	CITY OF CUTHBERT	RANDOLPH	GA	$6,559.41	1978	1982	Development
-419 - XXX	FLEMING PARK	RICHMOND COUNTY	RICHMOND	GA	$303,000.00	1978	1982	Development
-452 - XXX	RICHARDSON &amp; MILSTEAD PARKS	ROCKDALE COUNTY	ROCKDALE	GA	$39,100.89	1978	1983	Combination
-432 - XXX	ANDERSONVILLE NEIGHBORHOOD PARK	CITY OF ANDERSONVILLE	SUMTER	GA	$9,940.58	1978	1980	Development
-436 - XXX	MYERS PARK DEVELOPMENT	CITY OF AMERICUS	SUMTER	GA	$7,662.82	1978	1980	Development
-463 - XXX	GLENNVILLE PARK ACQ.	CITY OF GLENNVILLE	TATTNALL	GA	$20,200.00	1978	1983	Combination
-465 - XXX	THOMASVILLE GOLF COURSE	CITY OF THOMASVILLE	THOMAS	GA	$121,455.19	1978	1981	Development
-468 - XXX	UNION COUNTY PARK	UNION COUNTY	UNION	GA	$40,400.00	1978	1980	Acquisition
-423 - XXX	LAFAYETTE PARKS	CITY OF LAFAYETTE	WALKER	GA	$18,389.68	1978	1980	Development
-455 - XXX	WASHINGTON-WILKES RECREATION CENTER	CITY OF WASHINGTON &amp; WILKES COUNTY	WILKES	GA	$30,474.00	1978	1980	Development
-477 - E1	STATEWIDE FY 1979 CONSOLIDATED GRANT	APPLING COUNTY	APPLING	GA	$30,550.05	1979	1984	Development
-477 - G1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF WILLACOOCHEE	ATKINSON	GA	$10,123.46	1979	1984	Development
-477 - D	LITTLE FISHING CREEK GOLF COURSE	CITY OF MILLEDGEVILLE-BALDWIN COUNTY	BALDWIN	GA	$339,260.07	1979	1984	Development
-477 - T	STATEWIDE FY 1979 CONSOLIDATED GRANT	BARROW COUNTY	BARROW	GA	$42,897.08	1979	1984	Development
-477 - W	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF CARTERSVILLE	BARTOW	GA	$7,648.50	1979	1984	Development
-477 - M	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF RAY CITY	BERRIEN	GA	$19,962.98	1979	1984	Development
-477 - Q2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF MACON	BIBB	GA	$65,930.07	1979	1984	Development
-479 - XXX	OCMULGEE EAST PARK	CITY OF MACON	BIBB	GA	$136,350.00	1979	1982	Acquisition
-492 - XXX	METTER-CANDLER COUNTY PARK	CITY OF METTER &amp; CANDLER COUNTY	CANDLER	GA	$107,809.56	1979	1984	Combination
-475 - XXX	LAKE MAYER COMMUNITY PARK	CHATHAM COUNTY	CHATHAM	GA	$37,584.60	1979	1983	Development
-477 - E	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF TYBEE ISLAND	CHATHAM	GA	$63,207.09	1979	1984	Development
-477 - C2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF SAVANNAH	CHATHAM	GA	$102,000.00	1979	1984	Redevelopment
-477 - R2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CHATHAM COUNTY	CHATHAM	GA	$10,614.63	1979	1984	Development
-477 - G2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF SUMMERVILLE	CHATTOOGA	GA	$25,000.00	1979	1984	Development
-477 - X	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF CANTON	CHEROKEE	GA	$25,358.15	1979	1984	Development
-477 - L1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CLARKE COUNTY	CLARKE	GA	$19,172.70	1979	1984	Combination
-477 - M1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF COLLEGE PARK	CLAYTON	GA	$22,085.66	1979	1984	Development
-477 - P2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CLAYTON COUNTY	CLAYTON	GA	$53,339.38	1979	1984	Development
-477 - W1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CLAYTON COUNTY	CLAYTON	GA	$3,063.44	1979	1984	Development
-477 - X1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CLAYTON COUNTY	CLAYTON	GA	$50,577.45	1979	1984	Development
-477 - Y1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CLAYTON COUNTY	CLAYTON	GA	$19,914.24	1979	1984	Development
-477 - Z1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF FOREST PARK	CLAYTON	GA	$10,335.82	1979	1984	Acquisition
-476 - XXX	AL BISHOP SOFTBALL COMPLEX	COBB COUNTY	COBB	GA	$303,128.00	1979	1983	Development
-477 - U	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF MARIETTA	COBB	GA	$20,389.95	1979	1984	Development
-477 - A	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF DOUGLAS	COFFEE	GA	$40,792.00	1979	1984	Development
-477 - Y	STATEWIDE FY 1979 CONSOLIDATED GRANT	COWETA COUNTY	COWETA	GA	$24,321.18	1979	1984	Development
-477 - R1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF CORDELE	CRISP	GA	$71,160.94	1979	1984	Development
-477 - K1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF BAINBRIDGE	DECATUR	GA	$44,351.60	1979	1984	Development
-477 - V	STATEWIDE FY 1979 CONSOLIDATED GRANT	DEKALB COUNTY	DEKALB	GA	$658,683.58	1979	1984	Development
-477 - N1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF DECATUR	DEKALB	GA	$80,200.19	1979	1984	Development
-477 - P1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF STONE MOUNTAIN	DEKALB	GA	$93,663.20	1979	1984	Combination
-477 - H	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF VIENNA	DOOLY	GA	$9,673.79	1979	1984	Development
-477 - C1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF UNADILLA	DOOLY	GA	$7,731.88	1979	1984	Development
-477 - M2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF ALBANY	DOUGHERTY	GA	$84,532.38	1979	1984	Development
-477 - V1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF ADRIAN	EMANUEL	GA	$9,870.49	1979	1984	Development
-477 - N	STATEWIDE FY 1979 CONSOLIDATED GRANT	FAYETTE COUNTY	FAYETTE	GA	$40,844.51	1979	1984	Development
-477 - Q	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF PEACHTREE CITY	FAYETTE	GA	$10,707.92	1979	1984	Development
-466 - XXX	CASCADE SPRINGS NATURE PRESERVE	CITY OF ATLANTA	FULTON	GA	$493,885.06	1979	1981	Acquisition
-477 - T2	STATEWIDE FY 1979 CONSOLIDATED GRANT	FULTON COUNTY	FULTON	GA	$81,584.00	1979	1984	Acquisition
-477 - J	STATEWIDE FY 1979 CONSOLIDATED GRANT	GLYNN COUNTY	GLYNN	GA	$82,078.47	1979	1984	Development
-477 - J2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF GREENSBORO	GREENE	GA	$22,553.30	1979	1984	Development
-477 - B1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF SUGAR HILL	GWINNETT	GA	$41,236.02	1979	1984	Development
-477 - R	STATEWIDE FY 1979 CONSOLIDATED GRANT	HABERSHAM COUNTY	HABERSHAM	GA	$25,608.19	1979	1984	Redevelopment
-477 - Z	STATEWIDE FY 1979 CONSOLIDATED GRANT	HALL COUNTY	HALL	GA	$51,027.53	1979	1984	Development
-477 - I1	STATEWIDE FY 1979 CONSOLIDATED GRANT	HALL COUNTY	HALL	GA	$98,413.42	1979	1984	Development
-478 - XXX	TADMORE PARK	HALL COUNTY	HALL	GA	$85,373.91	1979	1982	Combination
-489 - XXX	LONGWOOD PARK	CITY OF GAINESVILLE	HALL	GA	$63,066.13	1979	1983	Combination
-477 - F	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF BREMEN	HARALSON	GA	$8,983.28	1979	1984	Development
-477 - D1	STATEWIDE FY 1979 CONSOLIDATED GRANT	HARRIS COUNTY	HARRIS	GA	$12,178.62	1979	1984	Development
-477 - J1	STATEWIDE FY 1979 CONSOLIDATED GRANT	HENRY COUNTY	HENRY	GA	$42,298.05	1979	1984	Development
-477 - A1	STATEWIDE FY 1979 CONSOLIDATED GRANT	JACKSON COUNTY	JACKSON	GA	$14,275.09	1979	1984	Combination
-477 - S2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF HAZLEHURST-JEFF DAVIS COUNTY	JEFF DAVIS	GA	$30,605.02	1979	1984	Combination
-477 - T1	STATEWIDE FY 1979 CONSOLIDATED GRANT	LAURENS COUNTY	LAURENS	GA	$3,841.04	1979	1984	Development
-485 - XXX	LAURENS - DEXTER PARK	LAURENS COUNTY	LAURENS	GA	$33,737.84	1979	1984	Combination
-480 - XXX	LINCOLN COUNTY PARK	LINCOLN COUNTY	LINCOLN	GA	$31,877.61	1979	1984	Combination
-477 - B	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF MOUNT VERNON	MONTGOMERY	GA	$18,895.70	1979	1984	Development
-477 - S	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF MADISON	MORGAN	GA	$20,363.58	1979	1984	Development
-484 - XXX	DNR FY79 ACQUISITION GRANT	DEPT. OF NATURAL RESOURCES	MULTI-COUNTY	GA	$2,139,698.94	1979	1985	Acquisition
-477 - A2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF COLUMBUS	MUSCOGEE	GA	$126,531.96	1979	1984	Combination
-477 - S1	STATEWIDE FY 1979 CONSOLIDATED GRANT	FLOYD COUNTY	MUSCOGEE	GA	$51,347.90	1979	1984	Development
-481 - XXX	SOUTH PEACH PARK ACQUISITION	FORT VALLEY REDEVELOPMENT AUTHORITY	PEACH	GA	$30,704.00	1979	1983	Acquisition
-486 - XXX	GEORGIA SCORP	DEPT. OF NATURAL RESOURCES	PLANNING	GA	$81,195.00	1979	1979	Planning
-477 - H1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF HAWKINSVILLE-PULASKI COUNTY	PULASKI	GA	$35,300.40	1979	1984	Development
-477 - I2	STATEWIDE FY 1979 CONSOLIDATED GRANT	ROCKDALE COUNTY	ROCKDALE	GA	$44,176.03	1979	1984	Combination
-477 - I	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF LUMPKIN	STEWART	GA	$15,302.89	1979	1984	Combination
-477 - P	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF REYNOLDS	TAYLOR	GA	$15,257.00	1979	1984	Development
-477 - L	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF THOMASVILLE	THOMAS	GA	$30,605.60	1979	1984	Combination
-477 - C	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF VIDALIA	TOOMBS	GA	$50,016.09	1979	1984	Redevelopment
-477 - F1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF LYONS	TOOMBS	GA	$40,792.00	1979	1984	Development
-477 - Q1	STATEWIDE FY 1979 CONSOLIDATED GRANT	TOWNS COUNTY	TOWNS	GA	$34,630.23	1979	1984	Development
-482 - XXX	WEST POINT PARK	CITY OF WEST POINT	TROUP	GA	$9,961.28	1979	1984	Combination
-477 - L2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF ASHBURN &amp; TURNER COUNTY	TURNER	GA	$30,377.60	1979	1984	Combination
-477 - B2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF SANDERSVILLE-WASHINGTON CO.	WASHINGTON	GA	$20,000.00	1979	1984	Development
-477 - N2	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF DALTON	WHITFIELD	GA	$28,764.15	1979	1984	Development
-477 - U1	STATEWIDE FY 1979 CONSOLIDATED GRANT	CITY OF ABBEVILLE	WILCOX	GA	$22,308.30	1979	1984	Combination
-513 - XXX	WILLACOOCHEE RECREATION PARK	CITY OF WILLACOOCHEE	ATKINSON	GA	$12,708.56	1980	1985	Development
-493 - C	NORTHSIDE PARK	CITY OF MACON	BIBB	GA	$101,868.67	1980	1985	Development
-493 - L	SANDY BEACH PARK 4	BIBB COUNTY	BIBB	GA	$25,413.86	1980	1985	Development
-512 - XXX	COCHRAN/BLECKLEY COUNTY PARK	CITY OF COCHRAN &amp; BLECKLEY COUNTY	BLECKLEY	GA	$19,863.31	1980	1985	Development
-488 - XXX	STATESBORO - BLITCH STREET PARK	CITY OF STATESBORO	BULLOCH	GA	$40,652.42	1980	1982	Development
-516 - XXX	HAMPTON L. DAUGHTRY PARK	CITY OF JACKSON-BUTTS COUNTY	BUTTS	GA	$20,131.31	1980	1985	Development
-493 - B1	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF ARLINGTON	CALHOUN	GA	$5,604.94	1980	1985	Development
-518 - XXX	WOODBINE CITY PARK	CAMDEN COUNTY	CAMDEN	GA	$77,415.14	1980	1985	Redevelopment
-493 - T	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF BOWDON	CARROLL	GA	$17,510.30	1980	1985	Development
-504 - XXX	GOLD DUST PARK	CITY OF VILLA RICA	CARROLL	GA	$78,679.64	1980	1985	Combination
-493 - A	GILBERT STEPHENSON PARK	CITY OF FORT OGLETHORPE	CATOOSA	GA	$18,743.37	1980	1985	Development
-493 - S	STATEWIDE FY 1980 CONSOLIDATED GRANT	CHATHAM COUNTY	CHATHAM	GA	$43,460.73	1980	1985	Development
-493 - E1	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF WINTERVILLE	CLARKE	GA	$10,269.95	1980	1985	Development
-493 - Q	STATEWIDE FY 1980 CONSOLIDATED GRANT	CLAYTON COUNTY	CLAYTON	GA	$89,461.59	1980	1985	Development
-493 - P	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF DOUGLAS	COFFEE	GA	$40,792.00	1980	1985	Development
-514 - XXX	BROXTON RECREATION PARK	CITY OF BROXTON	COFFEE	GA	$30,626.12	1980	1985	Combination
-501 - XXX	HARLEM PARK	COLUMBIA COUNTY	COLUMBIA	GA	$13,508.24	1980	1983	Development
-508 - XXX	APPLING PARK - PHASE II	COLUMBIA COUNTY	COLUMBIA	GA	$13,980.18	1980	1985	Development
-526 - XXX	MARTINEZ/REED CREEK PARK	COLUMBIA COUNTY	COLUMBIA	GA	$61,966.53	1980	1984	Combination
-510 - XXX	CENTRAL CITY PARK	CITY OF ATLANTA	DAWSON	GA	$323,657.00	1980	1985	Redevelopment
-493 - R	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF DECATUR	DEKALB	GA	$37,148.40	1980	1985	Development
-523 - XXX	FORT CREEK MOUNTAIN	DEKALB COUNTY	DEKALB	GA	$31,237.50	1980	1984	Acquisition
-532 - XXX	SHOAL CREEK &amp; DEARBORN PARKS	DEKALB COUNTY	DEKALB	GA	$69,357.42	1980	1985	Combination
-535 - XXX	MASON MILL AND BLACKBURN PARKS	DEKALB COUNTY	DEKALB	GA	$81,599.52	1980	1985	Development
-493 - V	CHEHAW PARK	CITY OF ALBANY	DOUGHERTY	GA	$15,243.64	1980	1985	Development
-494 - XXX	HUNTER MEMORIAL PARK	CITY OF DOUGLASVILLE	DOUGLAS	GA	$37,330.65	1980	1984	Acquisition
-493 - I1	STATEWIDE FY 1980 CONSOLIDATED GRANT	ECHOLS COUNTY	ECHOLS	GA	$25,745.93	1980	1985	Development
-519 - XXX	McCURRY PARK	FAYETTE COUNTY	FAYETTE	GA	$92,614.34	1980	1985	Development
-529 - XXX	SHAMROCK PARK (TYRONE REC. AREA)	FAYETTE COUNTY/CITY OF TYRONE	FAYETTE	GA	$23,489.57	1980	1985	Development
-522 - XXX	BENNETT MEMORIAL PARK	FORSYTH COUNTY	FORSYTH	GA	$30,598.39	1980	1985	Combination
-493 - J	STATEWIDE FY 1980 CONSOLIDATED GRANT	FULTON COUNTY	FULTON	GA	$64,247.40	1980	1985	Acquisition
-509 - XXX	SOUTHSIDE AND CENTER HILL PARKS	CITY OF ATLANTA	FULTON	GA	$114,350.31	1980	1985	Development
-521 - XXX	ALPHARETTA CITY PARK	CITY OF ALPHARETTA	FULTON	GA	$5,000.00	1980	1985	Development
-525 - XXX	RIDGEVIEW PARK	CITY OF SANDY SPRINGS	FULTON	GA	$50,652.59	1980	1985	Development
-536 - XXX	EAST ROSWELL PARK	CITY OF ROSWELL	FULTON	GA	$101,580.00	1980	1985	Acquisition
-503 - XXX	GILMER COUNTY GOLF COURSE	GILMER COUNTY	GILMER	GA	$351,336.47	1980	1985	Combination
-493 - H	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF SNELLVILLE	GWINNETT	GA	$30,666.74	1980	1985	Development
-506 - XXX	GAINESVILLE SWIMMING FACILITY	CITY OF GAINESVILLE	HALL	GA	$309,938.32	1980	1985	Development
-511 - XXX	TALLEY MOUNTAIN RECREATION COMPLEX	CITY OF TALLAPOOSA	HARALSON	GA	$109,156.03	1980	1985	Acquisition
-493 - B	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF WARNER ROBINS	HOUSTON	GA	$30,957.00	1980	1985	Development
-493 - U	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF WARNER ROBINS	HOUSTON	GA	$30,726.06	1980	1985	Development
-493 - F1	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF WARNER ROBINS	HOUSTON	GA	$27,315.98	1980	1985	Development
-520 - XXX	IRWIN COUNTY PARK	CITY OF OCILLA-IRWIN COUNTY	IRWIN	GA	$30,183.98	1980	1985	Development
-534 - XXX	BRASELTON COMMUNITY PARK	CITY OF BRASELTON	JACKSON	GA	$25,249.65	1980	1985	Combination
-502 - XXX	STAFFORD MEMORIAL PARK	LIBERTY COUNTY	LIBERTY	GA	$63,750.00	1980	1985	Development
-493 - D	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF VALDOSTA	LOWNDES	GA	$49,378.23	1980	1985	Development
-527 - XXX	BUENA VISTA CITY PARK	CITY OF BUENA VISTA	MARION	GA	$20,782.25	1980	1985	Development
-505 - XXX	MCINTOSH COUNTY TWO PARKS	MCINTOSH COUNTY	MCINTOSH	GA	$157,783.19	1980	1985	Combination
-517 - XXX	SPRING CREEK PARK	CITY OF COLQUITT &amp; MILLER COUNTY	MILLER	GA	$8,360.01	1980	1985	Development
-493 - J1	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF BACONTON	MITCHELL	GA	$23,358.80	1980	1985	Combination
-496 - XXX	PELHAM SPORTS COMPLEX	CITY OF PELHAM	MITCHELL	GA	$50,551.18	1980	1984	Combination
-497 - XXX	FLOYD ROAD REGIONAL PK	CITY OF COLUMBUS	MUSCOGEE	GA	$127,457.50	1980	1984	Acquisition
-493 - K	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF BOGART	OCONEE	GA	$12,595.92	1980	1985	Acquisition
-493 - M	STATEWIDE FY 1980 CONSOLIDATED GRANT	PEACH COUNTY	PEACH	GA	$34,269.07	1980	1985	Development
-493 - N	STATEWIDE FY 1980 CONSOLIDATED GRANT	PEACH COUNTY	PEACH	GA	$15,297.00	1980	1985	Acquisition
-524 - XXX	GEORGIA SCORP	DEPT. OF NATURAL RESOURCES	PLANNING	GA	$81,927.62	1980	1980	Planning
-533 - XXX	GEORGIA SCORP	DEPT. OF NATURAL RESOURCES	PLANNING	GA	$83,832.54	1980	1981	Planning
-499 - XXX	AUGUSTA TENNIS CENTER	CITY OF AUGUSTA	RICHMOND	GA	$255,768.93	1980	1985	Development
-493 - E	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF AMERICUS	SUMTER	GA	$163,818.77	1980	1985	Development
-493 - Z	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF GLENNVILLE	TATTNALL	GA	$36,658.01	1980	1985	Development
-493 - W	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF MEIGS	THOMAS	GA	$5,275.98	1980	1985	Development
-493 - C1	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF THOMASVILLE	THOMAS	GA	$41,276.00	1980	1985	Development
-493 - Y	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF VIDALIA	TOOMBS	GA	$50,844.65	1980	1985	Development
-493 - G1	STATEWIDE FY 1980 CONSOLIDATED GRANT	TOOMBS COUNTY	TOOMBS	GA	$41,275.99	1980	1985	Combination
-515 - XXX	ASHBURN PARK	CITY OF ASHBURN &amp; TURNER COUNTY	TURNER	GA	$25,484.19	1980	1985	Development
-507 - XXX	ROSSVILLE COMMUNITY PARK	CITY OF ROSSVILLE	WALKER	GA	$35,368.85	1980	1985	Development
-493 - D1	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF SOCIAL CIRCLE	WALTON	GA	$19,965.04	1980	1985	Development
-493 - G	STATEWIDE FY 1980 CONSOLIDATED GRANT	CITY OF ABBEVILLE	WILCOX	GA	$8,679.89	1980	1985	Development
-553 - XXX	BAXLEY-NORTHSIDE PARK	CITY OF BAXLEY	APPLING	GA	$19,403.25	1981	1986	Development
-552 - XXX	OCMULGEE EAST PARK	CITY OF MACON	BIBB	GA	$116,802.24	1981	1986	Development
-573 - XXX	RICHMOND HILL PARK EXERCISE TRAIL	BRYAN COUNTY	BRYAN	GA	$3,897.20	1981	1986	Development
-588 - XXX	CAMDEN COUNTY - GUM BRANCH PARK	CAMDEN COUNTY	CAMDEN	GA	$61,819.46	1981	1986	Combination
-571 - XXX	L. SCOTT STELL PARK	CHATHAM COUNTY	CHATHAM	GA	$126,822.75	1981	1984	Development
-539 - XXX	PATAULA SHORES BOATRAMP	CLAY COUNTY	CLAY	GA	$14,390.58	1981	1986	Development
-563 - XXX	INTERNATIONAL CONVENTION CENTER PARK	CITY OF COLLEGE PARK	CLAYTON	GA	$102,187.47	1981	1986	Combination
-541 - A	STATEWIDE FY 81 CONSOLIDATED GRANT	CITY OF DOUGLAS	COFFEE	GA	$46,435.50	1981	1985	Development
-537 - XXX	BERLIN RECREATIONAL COMPLEX - PHASE	CITY OF BERLIN	COLQUITT	GA	$2,284.50	1981	1985	Development
-538 - XXX	WADE-WALKER &amp; DUNWOODY PARKS	DEKALB COUNTY	DEKALB	GA	$397,800.00	1981	1983	Acquisition
-540 - XXX	FLOWERS PARK	CITY OF DORAVILLE	DEKALB	GA	$51,595.00	1981	1986	Development
-575 - XXX	EBSTER PARK POOL	CITY OF DECATUR	DEKALB	GA	$100,196.99	1981	1986	Development
-579 - XXX	DEKALB COUNTY PARK REVITALIZATION 81	DEKALB COUNTY	DEKALB	GA	$308,521.81	1981	1986	Redevelopment
-541 - F	STATEWIDE FY 81 CONSOLIDATED GRANT	DODGE COUNTY	DODGE	GA	$55,794.98	1981	1985	Combination
-555 - XXX	DEER LICK PARK	DOUGLAS COUNTY	DOUGLAS	GA	$52,045.81	1981	1986	Development
-556 - XXX	BILL ARP PARK	DOUGLAS COUNTY	DOUGLAS	GA	$12,671.70	1981	1986	Development
-546 - XXX	CRANE STREET PARK	CITY OF ROME	FLOYD	GA	$51,502.13	1981	1986	Development
-561 - XXX	CHATTAHOOCHEE NATURE CENTER	FULTON COUNTY	FULTON	GA	$82,445.75	1981	1986	Acquisition
-569 - XXX	ATLANTA PLAYGROUND DEVELOPMENT	CITY OF ATLANTA	FULTON	GA	$87,703.90	1981	1984	Redevelopment
-578 - XXX	BLYTHE ISLAND PARK	GLYNN COUNTY	GLYNN	GA	$81,135.91	1981	1986	Development
-560 - XXX	BARBER PARK-PHASE I	GRADY COUNTY	GRADY	GA	$103,644.55	1981	1984	Combination
-551 - XXX	LILBURN CITY PARK	CITY OF LILBURN	GWINNETT	GA	$20,178.54	1981	1986	Development
-541 - D	STATEWIDE FY 81 CONSOLIDATED GRANT	HANCOCK COUNTY	HANCOCK	GA	$48,019.34	1981	1985	Development
-550 - XXX	BREMEN CITY PARK ON	CITY OF BREMEN	HARALSON	GA	$36,116.50	1981	1986	Acquisition
-570 - XXX	JESSE TANNER MEMORIAL PARK	CITY OF WARNER ROBINS	HOUSTON	GA	$20,460.91	1981	1986	Development
-558 - XXX	JEFFERSON COMMUNITY PARK	CITY OF JEFFERSON	JACKSON	GA	$13,137.41	1981	1986	Redevelopment
-543 - XXX	LOUISVILLE MULTI-PURPOSE PARK	JEFFERSON COUNTY	JEFFERSON	GA	$30,788.53	1981	1986	Development
-541 - C	STATEWIDE FY 81 CONSOLIDATED GRANT	CITY OF MONTROSE &amp; LAURENS COUNTY	LAURENS	GA	$2,192.79	1981	1985	Development
-586 - XXX	BUCKEYE PARK	CITY OF EAST DUBLIN &amp; LAURENS COUNTY	LAURENS	GA	$19,779.60	1981	1986	Acquisition
-585 - XXX	LONG COUNTY PUBLIC BOAT RAMP	LONG COUNTY	LONG	GA	$22,938.75	1981	1986	Combination
-549 - XXX	MANCHESTER CITY PARK (HARMON FIELD)	CITY OF MANCHESTER	MERIWETHER	GA	$25,000.00	1981	1986	Development
-564 - XXX	HIRAM (ACQUISITION)	CITY OF HIRAM	PAULDING	GA	$22,340.83	1981	1982	Acquisition
-589 - XXX	NORTH PEACH PARK	PEACH COUNTY	PEACH	GA	$25,800.00	1981	1986	Development
-541 - E	STATEWIDE FY 81 CONSOLIDATED GRANT	CITY OF BLACKSHEAR	PIERCE	GA	$40,826.47	1981	1985	Development
-587 - XXX	GEORGIA SCORP	DEPT. OF NATURAL RESOURCES	PLANNING	GA	$5,691.35	1981	1981	Planning
-590 - XXX	GEORGIA SCORP	DEPT. OF NATURAL RESOURCES	PLANNING	GA	$36,000.00	1981	1983	Planning
-580 - XXX	RABUN COUNTY PARK	RABUN COUNTY	RABUN	GA	$177,330.32	1981	1984	Combination
-541 - B	STATE CONSOLIDATED PROJECT - FY 1981	DEPT. OF NATURAL RESOURCES	TATTNALL	GA	$22,685.85	1981	1985	Development
-545 - XXX	BALFOUR PARK	CITY OF THOMASVILLE	THOMAS	GA	$40,250.27	1981	1986	Redevelopment
-576 - XXX	FRIENDLY CITY PARK	TIFT COUNTY	TIFT	GA	$77,392.50	1981	1986	Acquisition
-547 - XXX	HAMMOND DRIVE PARK	CITY OF MONROE	WALTON	GA	$30,889.55	1981	1986	Development
-595 - XXX	CARROLL COUNTY-MCINTOSH RESERVE	CARROLL COUNTY	CARROLL	GA	$50,987.07	1982	1987	Development
-566 - XXX	MORROW CITY PARK	CITY OF MORROW	CLAYTON	GA	$25,000.00	1982	1984	Acquisition
-581 - XXX	JIM MILLER PARKK	COBB COUNTY	COBB	GA	$208,185.82	1982	1986	Acquisition
-591 - XXX	DAWSON COUNTY PARK	DAWSON COUNTY	DAWSON	GA	$97,674.00	1982	1984	Combination
-582 - XXX	COCHRAN MILL PARK	CITY OF CHATTAHOOCHEE HILLS	FULTON	GA	$203,377.70	1982	1987	Combination
-554 - XXX	GLYNN COUNTY BIKE PATHS	GLYNN COUNTY	GLYNN	GA	$84,716.49	1982	1986	Development
-594 - XXX	JEKYLL ISLAND POOL AND BIKE TRAIL	JEKYLL ISLAND AUTHORITY	GLYNN	GA	$111,108.05	1982	1986	Development
-592 - XXX	VALDOSTA - SUNSET PARK	CITY OF VALDOSTA	LOWNDES	GA	$20,400.00	1982	1986	Development
-574 - XXX	FACTORY SHOALS PARK	CITY OF COVINGTON-NEWTON COUNTY	NEWTON	GA	$165,620.22	1982	1987	Combination
-593 - XXX	LAGRANGE CITY PARK	CITY OF LAGRANGE	TROUP	GA	$35,700.00	1982	1986	Redevelopment
-596 - XXX	DALTON GOLF COURSE IMPROVEMENTS	CITY OF DALTON	WHITFIELD	GA	$55,073.80	1982	1983	Redevelopment
-597 - XXX	WALTER B. WILLIAMS PARK - POOL	CITY OF MILLEDGEVILLE-BALDWIN COUNTY	BALDWIN	GA	$40,885.51	1983	1984	Redevelopment
-604 - A	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF CARTERSVILLE	BARTOW	GA	$51,269.37	1983	1988	Combination
-601 - R	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF MACON	BIBB	GA	$71,305.66	1983	1984	Development
-612 - XXX	FREEDOM PARK	CITY OF MACON	BIBB	GA	$21,766.28	1983	1988	Development
-605 - XXX	BRYAND COUNTY PARKS	BRYAN COUNTY	BRYAN	GA	$53,889.53	1983	1988	Development
-601 - V	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF METTER	CANDLER	GA	$23,989.50	1983	1984	Development
-604 - C	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF BLOOMINGDALE	CHATHAM	GA	$15,315.00	1983	1988	Development
-611 - XXX	LYERLY ANGUS MCLEOD PARK	CITY OF LYERLY	CHATTOOGA	GA	$10,210.00	1983	1988	Development
-603 - XXX	JIM MILLER PARK	COBB COUNTY	COBB	GA	$334,181.00	1983	1988	Development
-604 - E	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF ACWORTH	COBB	GA	$30,809.81	1983	1988	Redevelopment
-601 - B1	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF DOUGLAS	COFFEE	GA	$30,414.77	1983	1984	Development
-601 - A1	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF MOULTRIE	COLQUITT	GA	$15,309.24	1983	1984	Development
-601 - Y	STATEWIDE FY 83 CONSOLIDATED GRANT	COLUMBIA COUNTY	COLUMBIA	GA	$12,779.20	1983	1984	Development
-604 - B	STATEWIDE FY 83 CONSOLIDATED GRANT	DADE COUNTY	DADE	GA	$52,472.98	1983	1988	Acquisition
-601 - K	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF STONE MOUNTAIN	DEKALB	GA	$15,315.00	1983	1984	Development
-607 - XXX	UNADILLA HARMON PARK	CITY OF UNADILLA	DOOLY	GA	$15,468.15	1983	1988	Development
-604 - I	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF BLAKELY-EARLY COUNTY	EARLY	GA	$10,720.50	1983	1988	Development
-601 - U	STATEWIDE FY 83 CONSOLIDATED GRANT	EVANS COUNTY	EVANS	GA	$35,715.86	1983	1984	Development
-601 - A	STATEWIDE FY 83 CONSOLIDATED GRANT	FLOYD COUNTY	FLOYD	GA	$30,591.95	1983	1984	Development
-606 - XXX	ROME MADDOX TRACK	CITY OF ROME	FLOYD	GA	$20,420.00	1983	1988	Redevelopment
-604 - D	STATEWIDE FY 83 CONSOLIDATED GRANT	FORSYTH COUNTY	FORSYTH	GA	$25,525.00	1983	1988	Acquisition
-601 - H	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF ROSWELL	FULTON	GA	$20,420.00	1983	1984	Development
-610 - XXX	PIEDMONT PARK	CITY OF ATLANTA	FULTON	GA	$104,370.00	1983	1988	Development
-601 - L	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF UNION POINT	GREENE	GA	$28,715.02	1983	1984	Development
-601 - G	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF SNELLVILLE	GWINNETT	GA	$20,346.51	1983	1984	Development
-601 - I	STATEWIDE FY 83 CONSOLIDATED GRANT	GWINNETT COUNTY	GWINNETT	GA	$51,047.15	1983	1984	Development
-601 - E	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF CLARKESVILLE	HABERSHAM	GA	$4,936.54	1983	1984	Development
-604 - G	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF WAVERLY HALL	HARRIS	GA	$15,309.77	1983	1988	Development
-609 - XXX	ROZAR PARK	CITY OF PERRY	HOUSTON	GA	$20,413.90	1983	1988	Development
-602 - XXX	WRENS - TWIN LAKE PARK	CITY OF WRENS	JEFFERSON	GA	$15,300.00	1983	1986	Acquisition
-601 - P	STATEWIDE FY 83 CONSOLIDATED GRANT	JONES COUNTY	JONES	GA	$18,242.58	1983	1984	Development
-601 - X	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF VALDOSTA	LOWNDES	GA	$25,501.87	1983	1984	Development
-601 - T	STATEWIDE FY 83 CONSOLIDATED GRANT	MACON COUNTY	MACON	GA	$22,257.80	1983	1984	Development
-613 - XXX	DNR FY83 ACQUISITION GRANT	DEPT. OF NATURAL RESOURCES	MULTI-COUNTY	GA	$435,620.96	1983	1988	Acquisition
-604 - F	STATEWIDE FY 83 CONSOLIDATED GRANT	OCONEE COUNTY	OCONEE	GA	$25,546.49	1983	1988	Development
-601 - J	STATEWIDE FY 83 CONSOLIDATED GRANT	PEACH COUNTY	PEACH	GA	$30,604.17	1983	1984	Development
-601 - C1	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF BLACKSHEAR	PIERCE	GA	$25,623.83	1983	1984	Development
-598 - XXX	GEORGIA SCORP	DEPT. OF NATURAL RESOURCES	PLANNING	GA	$34,993.44	1983	1984	Planning
-601 - Z	STATEWIDE FY 83 CONSOLIDATED GRANT	RICHMOND COUNTY	RICHMOND	GA	$30,630.00	1983	1984	Development
-601 - F	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF TOCCOA	STEPHENS	GA	$20,420.00	1983	1984	Development
-601 - S	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF AMERICUS	SUMTER	GA	$20,416.43	1983	1984	Redevelopment
-601 - W	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF GLENNVILLE	TATTNALL	GA	$17,149.10	1983	1984	Development
-601 - Q	STATEWIDE FY 83 CONSOLIDATED GRANT	TIFT COUNTY	TIFT	GA	$45,929.50	1983	1984	Development
-604 - H	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF SOPERTON	TREUTLEN	GA	$10,304.50	1983	1988	Combination
-601 - M	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF LAGRANGE	TROUP	GA	$53,599.56	1983	1984	Development
-600 - XXX	UNION COUNTY GOLF COURSE EXPANSION	UNION COUNTY	UNION	GA	$29,580.00	1983	1985	Acquisition
-604 - J	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF WAYCROSS-WARE COUNTY	WARE	GA	$20,420.00	1983	1988	Development
-601 - B	STATEWIDE FY 83 CONSOLIDATED GRANT	WHITFIELD COUNTY	WHITFIELD	GA	$25,525.00	1983	1984	Development
-601 - C	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF DALTON	WHITFIELD	GA	$3,777.37	1983	1984	Development
-601 - D	STATEWIDE FY 83 CONSOLIDATED GRANT	CITY OF TUNNEL HILL	WHITFIELD	GA	$20,408.39	1983	1984	Development
-616 - XXX	FALLING ROCKS PARK	CITY OF BAXLEY &amp; APPLING COUNTY	APPLING	GA	$41,890.41	1984	1988	Combination
-623 - E	STATEWIDE FY 84 CONSOLIDATED III	CITY OF MACON	BIBB	GA	$56,855.37	1984	1987	Development
-623 - B	STATEWIDE FY 84 CONSOLIDATED III	CAMDEN COUNTY	CAMDEN	GA	$25,877.42	1984	1987	Development
-622 - XXX	HULL PARK	CITY OF SAVANNAH	CHATHAM	GA	$62,160.08	1984	1987	Redevelopment
-621 - I	STATEWIDE FY84 CONSOLIDATED GRANT II	CITY OF SUMMERVILLE	CHATTOOGA	GA	$25,975.00	1984	1987	Development
-619 - C	W.L. DUPREE PARK	CITY OF WOODSTOCK	CHEROKEE	GA	$21,745.05	1984	1987	Development
-619 - D	STATEWIDE FY84 CONSOLIDATED GRANT	CITY OF CANTON	CHEROKEE	GA	$12,670.32	1984	1987	Development
-614 - XXX	SANDY CREEK GREENWAY	CLARKE COUNTY	CLARKE	GA	$20,420.00	1984	1984	Acquisition
-625 - B	STATEWIDE FY84 CONSOLIDATED GRANT IV	CLAYTON COUNTY	CLAYTON	GA	$16,879.99	1984	1987	Development
-625 - A	STATEWIDE FY84 CONSOLIDATED GRANT IV	CITY OF MARIETTA	COBB	GA	$43,657.28	1984	1987	Development
-625 - H	STATEWIDE FY84 CONSOLIDATED GRANT IV	DEKALB COUNTY	DEKALB	GA	$72,729.99	1984	1987	Acquisition
-625 - D	STATEWIDE FY84 CONSOLIDATED GRANT IV	CITY OF ALBANY	DOUGHERTY	GA	$13,283.82	1984	1987	Development
-625 - F	STATEWIDE FY84 CONSOLIDATED GRANT IV	DOUGHERTY COUNTY	DOUGHERTY	GA	$17,663.00	1984	1987	Development
-625 - I	STATEWIDE FY84 CONSOLIDATED GRANT IV	CITY OF ALBANY	DOUGHERTY	GA	$17,663.00	1984	1987	Development
-621 - A	STATEWIDE FY84 CONSOLIDATED GRANT II	CITY OF DOUGLASVILLE	DOUGLAS	GA	$20,828.11	1984	1987	Redevelopment
-619 - H	STATEWIDE FY84 CONSOLIDATED GRANT	CITY OF BOWMAN	ELBERT	GA	$20,456.00	1984	1987	Development
-621 - F	STATEWIDE FY84 CONSOLIDATED GRANT II	CITY OF SWAINSBORO	EMANUEL	GA	$20,420.00	1984	1987	Development
-621 - D	STATEWIDE FY84 CONSOLIDATED GRANT II	FAYETTE COUNTY	FAYETTE	GA	$12,383.07	1984	1987	Development
-619 - B	STATEWIDE FY84 CONSOLIDATED GRANT	FLOYD COUNTY	FLOYD	GA	$30,657.00	1984	1987	Development
-619 - F	STATEWIDE FY84 CONSOLIDATED GRANT	CITY OF CUMMING	FORSYTH	GA	$46,755.00	1984	1987	Redevelopment
-627 - XXX	PIEDMONT PARK	CITY OF ATLANTA	FULTON	GA	$103,317.85	1984	1987	Redevelopment
-629 - XXX	GRANT PARK - ATLANTA ZOO	CITY OF ATLANTA	FULTON	GA	$105,330.00	1984	1987	Redevelopment
-623 - A	STATEWIDE FY 84 CONSOLIDATED III	CITY OF BRUNSWICK	GLYNN	GA	$25,820.41	1984	1987	Development
-625 - E	STATEWIDE FY84 CONSOLIDATED GRANT IV	GLYNN COUNTY	GLYNN	GA	$74,559.38	1984	1987	Development
-626 - XXX	JEKYLL ISLAND PICNIC AREA	JEKYLL ISLAND AUTHORITY	GLYNN	GA	$71,448.86	1984	1987	Redevelopment
-628 - XXX	CALHOUN-GORDON RECREATION PARK	CITY OF CALHOUN	GORDON	GA	$30,785.54	1984	1987	Development
-619 - G	STATEWIDE FY84 CONSOLIDATED GRANT	CITY OF SUGAR HILL	GWINNETT	GA	$27,784.26	1984	1987	Development
-625 - C	STATEWIDE FY84 CONSOLIDATED GRANT IV	JOHNSON COUNTY	JOHNSON	GA	$20,575.70	1984	1987	Combination
-617 - XXX	BUCKEYE PARK	CITY OF EAST DUBLIN	LAURENS	GA	$10,390.00	1984	1988	Development
-621 - B	STATEWIDE FY84 CONSOLIDATED GRANT II	MADISON COUNTY	MADISON	GA	$20,904.20	1984	1987	Development
-625 - G	STATEWIDE FY84 CONSOLIDATED GRANT IV	MCDUFFIE COUNTY	MCDUFFIE	GA	$10,390.00	1984	1987	Development
-491 - XXX	DNR FY80/81 ACQUISITION GRANT	DEPT. OF NATURAL RESOURCES	MULTI-COUNTY	GA	$4,681,389.71	1984	1986	Acquisition
-623 - D	STATEWIDE FY 84 CONSOLIDATED </t>
-  </si>
-  <si>
-    <t>III</t>
-  </si>
-  <si>
     <t>621 - G</t>
   </si>
   <si>
@@ -5361,6 +5026,12 @@
   </si>
   <si>
     <t>WESTSIDE PARK-MIRACLE LEAGUE FIELD</t>
+  </si>
+  <si>
+    <t>BILL MORRIS PARK</t>
+  </si>
+  <si>
+    <t>623 - D</t>
   </si>
 </sst>
 </file>
@@ -5416,14 +5087,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -16102,49 +15770,72 @@
       <c r="A358" t="s">
         <v>250</v>
       </c>
-      <c r="B358" s="4" t="s">
-        <v>1296</v>
-      </c>
-      <c r="F358" s="2"/>
+      <c r="B358" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C358" t="s">
+        <v>968</v>
+      </c>
+      <c r="D358" t="s">
+        <v>969</v>
+      </c>
+      <c r="E358" t="s">
+        <v>750</v>
+      </c>
+      <c r="F358" s="2">
+        <v>20200</v>
+      </c>
+      <c r="G358">
+        <v>1977</v>
+      </c>
+      <c r="H358">
+        <v>1979</v>
+      </c>
+      <c r="I358" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>1297</v>
+        <v>1668</v>
       </c>
       <c r="B359" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C359" t="s">
         <v>888</v>
       </c>
-      <c r="C359" t="s">
+      <c r="D359" t="s">
         <v>806</v>
       </c>
-      <c r="D359" t="s">
-        <v>750</v>
-      </c>
-      <c r="E359" s="2">
+      <c r="E359" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="F359" s="2">
         <v>27574.77</v>
       </c>
-      <c r="F359" s="2">
+      <c r="G359">
         <v>1984</v>
       </c>
-      <c r="G359">
+      <c r="H359">
         <v>1987</v>
       </c>
-      <c r="H359" t="s">
+      <c r="I359" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B360" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C360" t="s">
         <v>1298</v>
       </c>
-      <c r="B360" t="s">
+      <c r="D360" t="s">
         <v>1299</v>
-      </c>
-      <c r="C360" t="s">
-        <v>1300</v>
-      </c>
-      <c r="D360" t="s">
-        <v>1301</v>
       </c>
       <c r="E360" t="s">
         <v>750</v>
@@ -16193,10 +15884,10 @@
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="B362" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="C362" t="s">
         <v>770</v>
@@ -16222,10 +15913,10 @@
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="B363" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="C363" t="s">
         <v>894</v>
@@ -16251,10 +15942,10 @@
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="B364" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="C364" t="s">
         <v>1145</v>
@@ -16280,10 +15971,10 @@
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="B365" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="C365" t="s">
         <v>333</v>
@@ -16312,10 +16003,10 @@
         <v>407</v>
       </c>
       <c r="B366" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="C366" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="D366" t="s">
         <v>1217</v>
@@ -16338,13 +16029,13 @@
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B367" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C367" t="s">
         <v>1309</v>
-      </c>
-      <c r="B367" t="s">
-        <v>1310</v>
-      </c>
-      <c r="C367" t="s">
-        <v>1311</v>
       </c>
       <c r="D367" t="s">
         <v>966</v>
@@ -16367,13 +16058,13 @@
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B368" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C368" t="s">
         <v>1312</v>
-      </c>
-      <c r="B368" t="s">
-        <v>1313</v>
-      </c>
-      <c r="C368" t="s">
-        <v>1314</v>
       </c>
       <c r="D368" t="s">
         <v>678</v>
@@ -16396,13 +16087,13 @@
     </row>
     <row r="369" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="B369" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="C369" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="D369" t="s">
         <v>812</v>
@@ -16425,16 +16116,16 @@
     </row>
     <row r="370" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B370" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C370" t="s">
         <v>1317</v>
       </c>
-      <c r="B370" t="s">
+      <c r="D370" t="s">
         <v>1318</v>
-      </c>
-      <c r="C370" t="s">
-        <v>1319</v>
-      </c>
-      <c r="D370" t="s">
-        <v>1320</v>
       </c>
       <c r="E370" t="s">
         <v>750</v>
@@ -16457,10 +16148,10 @@
         <v>412</v>
       </c>
       <c r="B371" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="C371" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="D371" t="s">
         <v>752</v>
@@ -16483,10 +16174,10 @@
     </row>
     <row r="372" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="B372" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="C372" t="s">
         <v>775</v>
@@ -16515,10 +16206,10 @@
         <v>423</v>
       </c>
       <c r="B373" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C373" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="D373" t="s">
         <v>690</v>
@@ -16544,10 +16235,10 @@
         <v>419</v>
       </c>
       <c r="B374" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="C374" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="D374" t="s">
         <v>690</v>
@@ -16570,10 +16261,10 @@
     </row>
     <row r="375" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="B375" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="C375" t="s">
         <v>1092</v>
@@ -16602,7 +16293,7 @@
         <v>422</v>
       </c>
       <c r="B376" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="C376" t="s">
         <v>328</v>
@@ -16628,10 +16319,10 @@
     </row>
     <row r="377" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A377" s="3" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="B377" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="C377" t="s">
         <v>319</v>
@@ -16660,7 +16351,7 @@
         <v>413</v>
       </c>
       <c r="B378" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="C378" t="s">
         <v>1098</v>
@@ -16689,7 +16380,7 @@
         <v>420</v>
       </c>
       <c r="B379" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="C379" t="s">
         <v>658</v>
@@ -16747,10 +16438,10 @@
         <v>409</v>
       </c>
       <c r="B381" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="C381" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="D381" t="s">
         <v>796</v>
@@ -16773,10 +16464,10 @@
     </row>
     <row r="382" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="B382" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="C382" t="s">
         <v>822</v>
@@ -16802,10 +16493,10 @@
     </row>
     <row r="383" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="B383" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="C383" t="s">
         <v>936</v>
@@ -16834,10 +16525,10 @@
         <v>414</v>
       </c>
       <c r="B384" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="C384" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="D384" t="s">
         <v>881</v>
@@ -16863,7 +16554,7 @@
         <v>659</v>
       </c>
       <c r="B385" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="C385" t="s">
         <v>883</v>
@@ -16892,7 +16583,7 @@
         <v>404</v>
       </c>
       <c r="B386" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="C386" t="s">
         <v>738</v>
@@ -16918,10 +16609,10 @@
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="B387" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="C387" t="s">
         <v>885</v>
@@ -16950,7 +16641,7 @@
         <v>662</v>
       </c>
       <c r="B388" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="C388" t="s">
         <v>885</v>
@@ -16976,13 +16667,13 @@
     </row>
     <row r="389" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="B389" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="C389" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D389" t="s">
         <v>315</v>
@@ -17005,16 +16696,16 @@
     </row>
     <row r="390" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B390" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C390" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D390" t="s">
         <v>1345</v>
-      </c>
-      <c r="B390" t="s">
-        <v>1335</v>
-      </c>
-      <c r="C390" t="s">
-        <v>1346</v>
-      </c>
-      <c r="D390" t="s">
-        <v>1347</v>
       </c>
       <c r="E390" t="s">
         <v>750</v>
@@ -17037,7 +16728,7 @@
         <v>411</v>
       </c>
       <c r="B391" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="C391" t="s">
         <v>1061</v>
@@ -17066,7 +16757,7 @@
         <v>418</v>
       </c>
       <c r="B392" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="C392" t="s">
         <v>1006</v>
@@ -17095,7 +16786,7 @@
         <v>405</v>
       </c>
       <c r="B393" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="C393" t="s">
         <v>1122</v>
@@ -17124,7 +16815,7 @@
         <v>408</v>
       </c>
       <c r="B394" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="C394" t="s">
         <v>888</v>
@@ -17150,16 +16841,16 @@
     </row>
     <row r="395" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B395" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C395" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D395" t="s">
         <v>1350</v>
-      </c>
-      <c r="B395" t="s">
-        <v>1335</v>
-      </c>
-      <c r="C395" t="s">
-        <v>1351</v>
-      </c>
-      <c r="D395" t="s">
-        <v>1352</v>
       </c>
       <c r="E395" t="s">
         <v>750</v>
@@ -17182,7 +16873,7 @@
         <v>660</v>
       </c>
       <c r="B396" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="C396" t="s">
         <v>1021</v>
@@ -17211,7 +16902,7 @@
         <v>424</v>
       </c>
       <c r="B397" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="C397" t="s">
         <v>1145</v>
@@ -17240,7 +16931,7 @@
         <v>410</v>
       </c>
       <c r="B398" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="C398" t="s">
         <v>333</v>
@@ -17266,13 +16957,13 @@
     </row>
     <row r="399" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B399" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="C399" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D399" t="s">
         <v>1030</v>
@@ -17298,7 +16989,7 @@
         <v>417</v>
       </c>
       <c r="B400" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="C400" t="s">
         <v>734</v>
@@ -17353,10 +17044,10 @@
     </row>
     <row r="402" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="B402" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="C402" t="s">
         <v>707</v>
@@ -17382,13 +17073,13 @@
     </row>
     <row r="403" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="B403" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="C403" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="D403" t="s">
         <v>969</v>
@@ -17414,10 +17105,10 @@
         <v>421</v>
       </c>
       <c r="B404" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="C404" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="D404" t="s">
         <v>812</v>
@@ -17443,13 +17134,13 @@
         <v>661</v>
       </c>
       <c r="B405" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C405" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D405" t="s">
         <v>1363</v>
-      </c>
-      <c r="C405" t="s">
-        <v>1364</v>
-      </c>
-      <c r="D405" t="s">
-        <v>1365</v>
       </c>
       <c r="E405" t="s">
         <v>750</v>
@@ -17472,7 +17163,7 @@
         <v>435</v>
       </c>
       <c r="B406" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="C406" t="s">
         <v>910</v>
@@ -17501,7 +17192,7 @@
         <v>427</v>
       </c>
       <c r="B407" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="C407" t="s">
         <v>775</v>
@@ -17530,7 +17221,7 @@
         <v>432</v>
       </c>
       <c r="B408" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="C408" t="s">
         <v>328</v>
@@ -17559,7 +17250,7 @@
         <v>429</v>
       </c>
       <c r="B409" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="C409" t="s">
         <v>339</v>
@@ -17588,10 +17279,10 @@
         <v>449</v>
       </c>
       <c r="B410" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C410" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="D410" t="s">
         <v>1254</v>
@@ -17617,10 +17308,10 @@
         <v>436</v>
       </c>
       <c r="B411" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="C411" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="D411" t="s">
         <v>796</v>
@@ -17646,10 +17337,10 @@
         <v>428</v>
       </c>
       <c r="B412" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="C412" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="D412" t="s">
         <v>685</v>
@@ -17678,7 +17369,7 @@
         <v>240</v>
       </c>
       <c r="C413" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D413" t="s">
         <v>315</v>
@@ -17704,7 +17395,7 @@
         <v>433</v>
       </c>
       <c r="B414" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="C414" t="s">
         <v>1204</v>
@@ -17733,7 +17424,7 @@
         <v>430</v>
       </c>
       <c r="B415" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="C415" t="s">
         <v>737</v>
@@ -17762,7 +17453,7 @@
         <v>426</v>
       </c>
       <c r="B416" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="C416" t="s">
         <v>740</v>
@@ -17878,7 +17569,7 @@
         <v>437</v>
       </c>
       <c r="B420" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="C420" t="s">
         <v>791</v>
@@ -17907,10 +17598,10 @@
         <v>451</v>
       </c>
       <c r="B421" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="C421" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="D421" t="s">
         <v>908</v>
@@ -17936,10 +17627,10 @@
         <v>454</v>
       </c>
       <c r="B422" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="C422" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="D422" t="s">
         <v>977</v>
@@ -17965,7 +17656,7 @@
         <v>440</v>
       </c>
       <c r="B423" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="C423" t="s">
         <v>775</v>
@@ -18023,7 +17714,7 @@
         <v>450</v>
       </c>
       <c r="B425" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="C425" t="s">
         <v>798</v>
@@ -18052,10 +17743,10 @@
         <v>666</v>
       </c>
       <c r="B426" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="C426" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="D426" t="s">
         <v>334</v>
@@ -18081,13 +17772,13 @@
         <v>444</v>
       </c>
       <c r="B427" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C427" t="s">
+        <v>1384</v>
+      </c>
+      <c r="D427" t="s">
         <v>1385</v>
-      </c>
-      <c r="C427" t="s">
-        <v>1386</v>
-      </c>
-      <c r="D427" t="s">
-        <v>1387</v>
       </c>
       <c r="E427" t="s">
         <v>750</v>
@@ -18110,7 +17801,7 @@
         <v>447</v>
       </c>
       <c r="B428" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="C428" t="s">
         <v>798</v>
@@ -18139,7 +17830,7 @@
         <v>434</v>
       </c>
       <c r="B429" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="C429" t="s">
         <v>995</v>
@@ -18168,10 +17859,10 @@
         <v>664</v>
       </c>
       <c r="B430" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="C430" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="D430" t="s">
         <v>881</v>
@@ -18197,10 +17888,10 @@
         <v>446</v>
       </c>
       <c r="B431" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="C431" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="D431" t="s">
         <v>1115</v>
@@ -18226,7 +17917,7 @@
         <v>445</v>
       </c>
       <c r="B432" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="C432" t="s">
         <v>1061</v>
@@ -18255,7 +17946,7 @@
         <v>665</v>
       </c>
       <c r="B433" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="C433" t="s">
         <v>1122</v>
@@ -18284,10 +17975,10 @@
         <v>663</v>
       </c>
       <c r="B434" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="C434" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="D434" t="s">
         <v>689</v>
@@ -18313,7 +18004,7 @@
         <v>448</v>
       </c>
       <c r="B435" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="C435" t="s">
         <v>333</v>
@@ -18342,7 +18033,7 @@
         <v>442</v>
       </c>
       <c r="B436" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="C436" t="s">
         <v>1032</v>
@@ -18371,7 +18062,7 @@
         <v>668</v>
       </c>
       <c r="B437" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="C437" t="s">
         <v>1065</v>
@@ -18400,10 +18091,10 @@
         <v>441</v>
       </c>
       <c r="B438" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="C438" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="D438" t="s">
         <v>969</v>
@@ -18429,13 +18120,13 @@
         <v>457</v>
       </c>
       <c r="B439" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C439" t="s">
+        <v>1399</v>
+      </c>
+      <c r="D439" t="s">
         <v>1400</v>
-      </c>
-      <c r="C439" t="s">
-        <v>1401</v>
-      </c>
-      <c r="D439" t="s">
-        <v>1402</v>
       </c>
       <c r="E439" t="s">
         <v>750</v>
@@ -18487,7 +18178,7 @@
         <v>671</v>
       </c>
       <c r="B441" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="C441" t="s">
         <v>1101</v>
@@ -18516,7 +18207,7 @@
         <v>667</v>
       </c>
       <c r="B442" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="C442" t="s">
         <v>855</v>
@@ -18545,10 +18236,10 @@
         <v>460</v>
       </c>
       <c r="B443" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="C443" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="D443" t="s">
         <v>932</v>
@@ -18574,7 +18265,7 @@
         <v>461</v>
       </c>
       <c r="B444" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="C444" t="s">
         <v>1051</v>
@@ -18603,7 +18294,7 @@
         <v>458</v>
       </c>
       <c r="B445" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="C445" t="s">
         <v>938</v>
@@ -18661,10 +18352,10 @@
         <v>459</v>
       </c>
       <c r="B447" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="C447" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D447" t="s">
         <v>315</v>
@@ -18690,10 +18381,10 @@
         <v>453</v>
       </c>
       <c r="B448" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="C448" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D448" t="s">
         <v>1030</v>
@@ -18748,7 +18439,7 @@
         <v>452</v>
       </c>
       <c r="B450" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="C450" t="s">
         <v>707</v>
@@ -18777,7 +18468,7 @@
         <v>462</v>
       </c>
       <c r="B451" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="C451" t="s">
         <v>907</v>
@@ -18806,7 +18497,7 @@
         <v>467</v>
       </c>
       <c r="B452" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="C452" t="s">
         <v>910</v>
@@ -18838,7 +18529,7 @@
         <v>735</v>
       </c>
       <c r="C453" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="D453" t="s">
         <v>752</v>
@@ -18864,7 +18555,7 @@
         <v>469</v>
       </c>
       <c r="B454" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="C454" t="s">
         <v>1233</v>
@@ -18893,10 +18584,10 @@
         <v>465</v>
       </c>
       <c r="B455" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="C455" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="D455" t="s">
         <v>778</v>
@@ -18922,7 +18613,7 @@
         <v>474</v>
       </c>
       <c r="B456" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="C456" t="s">
         <v>739</v>
@@ -18951,10 +18642,10 @@
         <v>485</v>
       </c>
       <c r="B457" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="C457" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="D457" t="s">
         <v>796</v>
@@ -19009,10 +18700,10 @@
         <v>464</v>
       </c>
       <c r="B459" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="C459" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="D459" t="s">
         <v>1199</v>
@@ -19038,7 +18729,7 @@
         <v>455</v>
       </c>
       <c r="B460" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="C460" t="s">
         <v>1001</v>
@@ -19067,7 +18758,7 @@
         <v>477</v>
       </c>
       <c r="B461" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="C461" t="s">
         <v>1264</v>
@@ -19096,7 +18787,7 @@
         <v>466</v>
       </c>
       <c r="B462" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="C462" t="s">
         <v>1117</v>
@@ -19125,10 +18816,10 @@
         <v>470</v>
       </c>
       <c r="B463" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="C463" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="D463" t="s">
         <v>693</v>
@@ -19154,7 +18845,7 @@
         <v>473</v>
       </c>
       <c r="B464" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="C464" t="s">
         <v>399</v>
@@ -19183,7 +18874,7 @@
         <v>468</v>
       </c>
       <c r="B465" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="C465" t="s">
         <v>737</v>
@@ -19212,7 +18903,7 @@
         <v>463</v>
       </c>
       <c r="B466" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="C466" t="s">
         <v>888</v>
@@ -19241,13 +18932,13 @@
         <v>471</v>
       </c>
       <c r="B467" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="C467" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="D467" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="E467" t="s">
         <v>750</v>
@@ -19270,10 +18961,10 @@
         <v>489</v>
       </c>
       <c r="B468" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="C468" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="D468" t="s">
         <v>377</v>
@@ -19299,7 +18990,7 @@
         <v>475</v>
       </c>
       <c r="B469" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="C469" t="s">
         <v>740</v>
@@ -19328,10 +19019,10 @@
         <v>673</v>
       </c>
       <c r="B470" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="C470" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="D470" t="s">
         <v>892</v>
@@ -19357,10 +19048,10 @@
         <v>479</v>
       </c>
       <c r="B471" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="C471" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="D471" t="s">
         <v>908</v>
@@ -19386,10 +19077,10 @@
         <v>486</v>
       </c>
       <c r="B472" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="C472" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="D472" t="s">
         <v>752</v>
@@ -19418,7 +19109,7 @@
         <v>729</v>
       </c>
       <c r="C473" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="D473" t="s">
         <v>1181</v>
@@ -19444,7 +19135,7 @@
         <v>490</v>
       </c>
       <c r="B474" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="C474" t="s">
         <v>339</v>
@@ -19502,7 +19193,7 @@
         <v>487</v>
       </c>
       <c r="B476" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="C476" t="s">
         <v>995</v>
@@ -19531,7 +19222,7 @@
         <v>480</v>
       </c>
       <c r="B477" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="C477" t="s">
         <v>883</v>
@@ -19560,7 +19251,7 @@
         <v>476</v>
       </c>
       <c r="B478" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="C478" t="s">
         <v>333</v>
@@ -19589,13 +19280,13 @@
         <v>674</v>
       </c>
       <c r="B479" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C479" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D479" t="s">
         <v>1363</v>
-      </c>
-      <c r="C479" t="s">
-        <v>1442</v>
-      </c>
-      <c r="D479" t="s">
-        <v>1365</v>
       </c>
       <c r="E479" t="s">
         <v>750</v>
@@ -19618,10 +19309,10 @@
         <v>501</v>
       </c>
       <c r="B480" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="C480" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="D480" t="s">
         <v>908</v>
@@ -19647,10 +19338,10 @@
         <v>484</v>
       </c>
       <c r="B481" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C481" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="D481" t="s">
         <v>690</v>
@@ -19676,7 +19367,7 @@
         <v>507</v>
       </c>
       <c r="B482" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="C482" t="s">
         <v>1092</v>
@@ -19705,7 +19396,7 @@
         <v>482</v>
       </c>
       <c r="B483" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="C483" t="s">
         <v>328</v>
@@ -19734,7 +19425,7 @@
         <v>500</v>
       </c>
       <c r="B484" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="C484" t="s">
         <v>339</v>
@@ -19763,7 +19454,7 @@
         <v>497</v>
       </c>
       <c r="B485" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="C485" t="s">
         <v>855</v>
@@ -19792,7 +19483,7 @@
         <v>483</v>
       </c>
       <c r="B486" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="C486" t="s">
         <v>798</v>
@@ -19821,7 +19512,7 @@
         <v>496</v>
       </c>
       <c r="B487" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="C487" t="s">
         <v>1001</v>
@@ -19850,7 +19541,7 @@
         <v>506</v>
       </c>
       <c r="B488" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="C488" t="s">
         <v>1117</v>
@@ -19908,7 +19599,7 @@
         <v>498</v>
       </c>
       <c r="B490" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="C490" t="s">
         <v>1122</v>
@@ -19937,7 +19628,7 @@
         <v>499</v>
       </c>
       <c r="B491" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="C491" t="s">
         <v>740</v>
@@ -19966,13 +19657,13 @@
         <v>675</v>
       </c>
       <c r="B492" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="C492" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="D492" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="E492" t="s">
         <v>750</v>
@@ -19995,7 +19686,7 @@
         <v>481</v>
       </c>
       <c r="B493" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="C493" t="s">
         <v>333</v>
@@ -20024,10 +19715,10 @@
         <v>493</v>
       </c>
       <c r="B494" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="C494" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D494" t="s">
         <v>1030</v>
@@ -20053,13 +19744,13 @@
         <v>495</v>
       </c>
       <c r="B495" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C495" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D495" t="s">
         <v>1454</v>
-      </c>
-      <c r="C495" t="s">
-        <v>1455</v>
-      </c>
-      <c r="D495" t="s">
-        <v>1456</v>
       </c>
       <c r="E495" t="s">
         <v>750</v>
@@ -20082,7 +19773,7 @@
         <v>539</v>
       </c>
       <c r="B496" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="C496" t="s">
         <v>1222</v>
@@ -20140,10 +19831,10 @@
         <v>511</v>
       </c>
       <c r="B498" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="C498" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="D498" t="s">
         <v>295</v>
@@ -20169,10 +19860,10 @@
         <v>536</v>
       </c>
       <c r="B499" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="C499" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="D499" t="s">
         <v>778</v>
@@ -20198,7 +19889,7 @@
         <v>540</v>
       </c>
       <c r="B500" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="C500" t="s">
         <v>339</v>
@@ -20227,7 +19918,7 @@
         <v>695</v>
       </c>
       <c r="B501" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="C501" t="s">
         <v>989</v>
@@ -20256,10 +19947,10 @@
         <v>492</v>
       </c>
       <c r="B502" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="C502" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="D502" t="s">
         <v>796</v>
@@ -20285,7 +19976,7 @@
         <v>517</v>
       </c>
       <c r="B503" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="C503" t="s">
         <v>1051</v>
@@ -20314,7 +20005,7 @@
         <v>505</v>
       </c>
       <c r="B504" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="C504" t="s">
         <v>1117</v>
@@ -20343,10 +20034,10 @@
         <v>696</v>
       </c>
       <c r="B505" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="C505" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="D505" t="s">
         <v>358</v>
@@ -20372,7 +20063,7 @@
         <v>509</v>
       </c>
       <c r="B506" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="C506" t="s">
         <v>1006</v>
@@ -20401,10 +20092,10 @@
         <v>510</v>
       </c>
       <c r="B507" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="C507" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="D507" t="s">
         <v>689</v>
@@ -20430,10 +20121,10 @@
         <v>541</v>
       </c>
       <c r="B508" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="C508" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="D508" t="s">
         <v>681</v>
@@ -20459,7 +20150,7 @@
         <v>494</v>
       </c>
       <c r="B509" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="C509" t="s">
         <v>740</v>
@@ -20488,7 +20179,7 @@
         <v>502</v>
       </c>
       <c r="B510" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="C510" t="s">
         <v>740</v>
@@ -20517,10 +20208,10 @@
         <v>508</v>
       </c>
       <c r="B511" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="C511" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="D511" t="s">
         <v>1152</v>
@@ -20546,10 +20237,10 @@
         <v>491</v>
       </c>
       <c r="B512" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="C512" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="D512" t="s">
         <v>687</v>
@@ -20575,10 +20266,10 @@
         <v>524</v>
       </c>
       <c r="B513" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="C513" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="D513" t="s">
         <v>908</v>
@@ -20662,7 +20353,7 @@
         <v>534</v>
       </c>
       <c r="B516" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="C516" t="s">
         <v>1222</v>
@@ -20720,10 +20411,10 @@
         <v>546</v>
       </c>
       <c r="B518" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="C518" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="D518" t="s">
         <v>817</v>
@@ -20749,7 +20440,7 @@
         <v>550</v>
       </c>
       <c r="B519" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="C519" t="s">
         <v>658</v>
@@ -20778,10 +20469,10 @@
         <v>552</v>
       </c>
       <c r="B520" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="C520" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="D520" t="s">
         <v>732</v>
@@ -20807,7 +20498,7 @@
         <v>514</v>
       </c>
       <c r="B521" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="C521" t="s">
         <v>1111</v>
@@ -20836,10 +20527,10 @@
         <v>519</v>
       </c>
       <c r="B522" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="C522" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="D522" t="s">
         <v>685</v>
@@ -20894,10 +20585,10 @@
         <v>551</v>
       </c>
       <c r="B524" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="C524" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="D524" t="s">
         <v>1115</v>
@@ -20923,13 +20614,13 @@
         <v>530</v>
       </c>
       <c r="B525" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="C525" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D525" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="E525" t="s">
         <v>750</v>
@@ -20952,7 +20643,7 @@
         <v>520</v>
       </c>
       <c r="B526" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="C526" t="s">
         <v>740</v>
@@ -20981,10 +20672,10 @@
         <v>697</v>
       </c>
       <c r="B527" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="C527" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="D527" t="s">
         <v>677</v>
@@ -21010,7 +20701,7 @@
         <v>528</v>
       </c>
       <c r="B528" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="C528" t="s">
         <v>333</v>
@@ -21039,10 +20730,10 @@
         <v>512</v>
       </c>
       <c r="B529" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="C529" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="D529" t="s">
         <v>908</v>
@@ -21068,10 +20759,10 @@
         <v>533</v>
       </c>
       <c r="B530" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="C530" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="D530" t="s">
         <v>395</v>
@@ -21097,10 +20788,10 @@
         <v>556</v>
       </c>
       <c r="B531" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="C531" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="D531" t="s">
         <v>796</v>
@@ -21126,7 +20817,7 @@
         <v>515</v>
       </c>
       <c r="B532" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="C532" t="s">
         <v>798</v>
@@ -21155,7 +20846,7 @@
         <v>516</v>
       </c>
       <c r="B533" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="C533" t="s">
         <v>877</v>
@@ -21184,7 +20875,7 @@
         <v>554</v>
       </c>
       <c r="B534" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="C534" t="s">
         <v>1001</v>
@@ -21242,7 +20933,7 @@
         <v>532</v>
       </c>
       <c r="B536" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="C536" t="s">
         <v>740</v>
@@ -21271,7 +20962,7 @@
         <v>549</v>
       </c>
       <c r="B537" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="C537" t="s">
         <v>740</v>
@@ -21300,7 +20991,7 @@
         <v>521</v>
       </c>
       <c r="B538" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="C538" t="s">
         <v>333</v>
@@ -21329,7 +21020,7 @@
         <v>547</v>
       </c>
       <c r="B539" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="C539" t="s">
         <v>740</v>
@@ -21387,10 +21078,10 @@
         <v>537</v>
       </c>
       <c r="B541" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="C541" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="D541" t="s">
         <v>57</v>
@@ -21416,7 +21107,7 @@
         <v>518</v>
       </c>
       <c r="B542" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="C542" t="s">
         <v>973</v>
@@ -21445,7 +21136,7 @@
         <v>513</v>
       </c>
       <c r="B543" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="C543" t="s">
         <v>1240</v>
@@ -21474,10 +21165,10 @@
         <v>526</v>
       </c>
       <c r="B544" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="C544" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D544" t="s">
         <v>736</v>
@@ -21503,10 +21194,10 @@
         <v>699</v>
       </c>
       <c r="B545" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="C545" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="D545" t="s">
         <v>782</v>
@@ -21532,10 +21223,10 @@
         <v>545</v>
       </c>
       <c r="B546" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="C546" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="D546" t="s">
         <v>728</v>
@@ -21561,10 +21252,10 @@
         <v>557</v>
       </c>
       <c r="B547" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="C547" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="D547" t="s">
         <v>1254</v>
@@ -21590,7 +21281,7 @@
         <v>555</v>
       </c>
       <c r="B548" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="C548" t="s">
         <v>877</v>
@@ -21619,7 +21310,7 @@
         <v>523</v>
       </c>
       <c r="B549" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="C549" t="s">
         <v>1261</v>
@@ -21648,7 +21339,7 @@
         <v>548</v>
       </c>
       <c r="B550" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="C550" t="s">
         <v>1117</v>
@@ -21677,7 +21368,7 @@
         <v>535</v>
       </c>
       <c r="B551" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="C551" t="s">
         <v>391</v>
@@ -21706,10 +21397,10 @@
         <v>700</v>
       </c>
       <c r="B552" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="C552" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="D552" t="s">
         <v>917</v>
@@ -21735,7 +21426,7 @@
         <v>538</v>
       </c>
       <c r="B553" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="C553" t="s">
         <v>1226</v>
@@ -21764,10 +21455,10 @@
         <v>553</v>
       </c>
       <c r="B554" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="C554" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="D554" t="s">
         <v>334</v>
@@ -21793,10 +21484,10 @@
         <v>566</v>
       </c>
       <c r="B555" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="C555" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="D555" t="s">
         <v>778</v>
@@ -21822,7 +21513,7 @@
         <v>718</v>
       </c>
       <c r="B556" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="C556" t="s">
         <v>658</v>
@@ -21851,7 +21542,7 @@
         <v>522</v>
       </c>
       <c r="B557" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="C557" t="s">
         <v>694</v>
@@ -21880,10 +21571,10 @@
         <v>561</v>
       </c>
       <c r="B558" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="C558" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="D558" t="s">
         <v>736</v>
@@ -21909,10 +21600,10 @@
         <v>559</v>
       </c>
       <c r="B559" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="C559" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="D559" t="s">
         <v>782</v>
@@ -21938,10 +21629,10 @@
         <v>527</v>
       </c>
       <c r="B560" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="C560" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="D560" t="s">
         <v>926</v>
@@ -21967,7 +21658,7 @@
         <v>709</v>
       </c>
       <c r="B561" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="C561" t="s">
         <v>1054</v>
@@ -21996,7 +21687,7 @@
         <v>543</v>
       </c>
       <c r="B562" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="C562" t="s">
         <v>738</v>
@@ -22025,7 +21716,7 @@
         <v>560</v>
       </c>
       <c r="B563" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="C563" t="s">
         <v>682</v>
@@ -22054,10 +21745,10 @@
         <v>564</v>
       </c>
       <c r="B564" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="C564" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="D564" t="s">
         <v>1062</v>
@@ -22083,7 +21774,7 @@
         <v>575</v>
       </c>
       <c r="B565" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="C565" t="s">
         <v>391</v>
@@ -22115,7 +21806,7 @@
         <v>767</v>
       </c>
       <c r="C566" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="D566" t="s">
         <v>768</v>
@@ -22141,7 +21832,7 @@
         <v>563</v>
       </c>
       <c r="B567" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="C567" t="s">
         <v>403</v>
@@ -22170,10 +21861,10 @@
         <v>574</v>
       </c>
       <c r="B568" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="C568" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="D568" t="s">
         <v>1148</v>
@@ -22199,7 +21890,7 @@
         <v>719</v>
       </c>
       <c r="B569" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="C569" t="s">
         <v>962</v>
@@ -22228,10 +21919,10 @@
         <v>576</v>
       </c>
       <c r="B570" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="C570" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="D570" t="s">
         <v>1159</v>
@@ -22257,10 +21948,10 @@
         <v>590</v>
       </c>
       <c r="B571" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="C571" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="D571" t="s">
         <v>334</v>
@@ -22289,7 +21980,7 @@
         <v>757</v>
       </c>
       <c r="C572" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="D572" t="s">
         <v>736</v>
@@ -22315,10 +22006,10 @@
         <v>583</v>
       </c>
       <c r="B573" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="C573" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
       <c r="D573" t="s">
         <v>736</v>
@@ -22344,7 +22035,7 @@
         <v>565</v>
       </c>
       <c r="B574" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="C574" t="s">
         <v>852</v>
@@ -22373,7 +22064,7 @@
         <v>573</v>
       </c>
       <c r="B575" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="C575" t="s">
         <v>305</v>
@@ -22402,10 +22093,10 @@
         <v>597</v>
       </c>
       <c r="B576" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="C576" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="D576" t="s">
         <v>782</v>
@@ -22431,10 +22122,10 @@
         <v>589</v>
       </c>
       <c r="B577" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="C577" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="D577" t="s">
         <v>926</v>
@@ -22460,10 +22151,10 @@
         <v>562</v>
       </c>
       <c r="B578" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="C578" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="D578" t="s">
         <v>929</v>
@@ -22492,7 +22183,7 @@
         <v>727</v>
       </c>
       <c r="C579" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="D579" t="s">
         <v>314</v>
@@ -22518,10 +22209,10 @@
         <v>568</v>
       </c>
       <c r="B580" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="C580" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="D580" t="s">
         <v>878</v>
@@ -22547,10 +22238,10 @@
         <v>569</v>
       </c>
       <c r="B581" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="C581" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="D581" t="s">
         <v>881</v>
@@ -22605,7 +22296,7 @@
         <v>577</v>
       </c>
       <c r="B583" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="C583" t="s">
         <v>741</v>
@@ -22634,10 +22325,10 @@
         <v>570</v>
       </c>
       <c r="B584" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
       <c r="C584" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="D584" t="s">
         <v>691</v>
@@ -22663,10 +22354,10 @@
         <v>724</v>
       </c>
       <c r="B585" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="C585" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="D585" t="s">
         <v>301</v>
@@ -22692,7 +22383,7 @@
         <v>579</v>
       </c>
       <c r="B586" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="C586" t="s">
         <v>1279</v>
@@ -22721,10 +22412,10 @@
         <v>578</v>
       </c>
       <c r="B587" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="C587" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="D587" t="s">
         <v>765</v>
@@ -22750,10 +22441,10 @@
         <v>715</v>
       </c>
       <c r="B588" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="C588" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="D588" t="s">
         <v>681</v>
@@ -22779,10 +22470,10 @@
         <v>716</v>
       </c>
       <c r="B589" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="C589" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="D589" t="s">
         <v>14</v>
@@ -22808,10 +22499,10 @@
         <v>582</v>
       </c>
       <c r="B590" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="C590" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="D590" t="s">
         <v>892</v>
@@ -22837,10 +22528,10 @@
         <v>572</v>
       </c>
       <c r="B591" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="C591" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="D591" t="s">
         <v>1148</v>
@@ -22866,10 +22557,10 @@
         <v>585</v>
       </c>
       <c r="B592" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="C592" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="D592" t="s">
         <v>728</v>
@@ -22895,10 +22586,10 @@
         <v>580</v>
       </c>
       <c r="B593" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="C593" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="D593" t="s">
         <v>685</v>
@@ -22924,10 +22615,10 @@
         <v>581</v>
       </c>
       <c r="B594" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="C594" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="D594" t="s">
         <v>348</v>
@@ -22953,10 +22644,10 @@
         <v>591</v>
       </c>
       <c r="B595" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="C595" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="D595" t="s">
         <v>1129</v>
@@ -22982,10 +22673,10 @@
         <v>594</v>
       </c>
       <c r="B596" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="C596" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="D596" t="s">
         <v>377</v>
@@ -23011,10 +22702,10 @@
         <v>702</v>
       </c>
       <c r="B597" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="C597" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="D597" t="s">
         <v>690</v>
@@ -23040,7 +22731,7 @@
         <v>592</v>
       </c>
       <c r="B598" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="C598" t="s">
         <v>1098</v>
@@ -23069,10 +22760,10 @@
         <v>598</v>
       </c>
       <c r="B599" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="C599" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="D599" t="s">
         <v>778</v>
@@ -23098,10 +22789,10 @@
         <v>595</v>
       </c>
       <c r="B600" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="C600" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="D600" t="s">
         <v>395</v>
@@ -23127,7 +22818,7 @@
         <v>599</v>
       </c>
       <c r="B601" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="C601" t="s">
         <v>1046</v>
@@ -23156,13 +22847,13 @@
         <v>721</v>
       </c>
       <c r="B602" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C602" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D602" t="s">
         <v>1587</v>
-      </c>
-      <c r="C602" t="s">
-        <v>1588</v>
-      </c>
-      <c r="D602" t="s">
-        <v>1589</v>
       </c>
       <c r="E602" t="s">
         <v>750</v>
@@ -23185,10 +22876,10 @@
         <v>586</v>
       </c>
       <c r="B603" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="C603" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="D603" t="s">
         <v>796</v>
@@ -23214,10 +22905,10 @@
         <v>605</v>
       </c>
       <c r="B604" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="C604" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="D604" t="s">
         <v>314</v>
@@ -23243,10 +22934,10 @@
         <v>701</v>
       </c>
       <c r="B605" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="C605" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="D605" t="s">
         <v>685</v>
@@ -23272,7 +22963,7 @@
         <v>596</v>
       </c>
       <c r="B606" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="C606" t="s">
         <v>1001</v>
@@ -23301,10 +22992,10 @@
         <v>723</v>
       </c>
       <c r="B607" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
       <c r="C607" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="D607" t="s">
         <v>803</v>
@@ -23330,10 +23021,10 @@
         <v>602</v>
       </c>
       <c r="B608" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="C608" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="D608" t="s">
         <v>315</v>
@@ -23359,7 +23050,7 @@
         <v>588</v>
       </c>
       <c r="B609" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="C609" t="s">
         <v>737</v>
@@ -23388,10 +23079,10 @@
         <v>593</v>
       </c>
       <c r="B610" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="C610" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="D610" t="s">
         <v>681</v>
@@ -23417,13 +23108,13 @@
         <v>584</v>
       </c>
       <c r="B611" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="C611" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="D611" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="E611" t="s">
         <v>750</v>
@@ -23446,10 +23137,10 @@
         <v>600</v>
       </c>
       <c r="B612" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="C612" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="D612" t="s">
         <v>383</v>
@@ -23475,7 +23166,7 @@
         <v>587</v>
       </c>
       <c r="B613" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="C613" t="s">
         <v>1019</v>
@@ -23504,10 +23195,10 @@
         <v>711</v>
       </c>
       <c r="B614" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="C614" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="D614" t="s">
         <v>892</v>
@@ -23533,7 +23224,7 @@
         <v>712</v>
       </c>
       <c r="B615" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="C615" t="s">
         <v>1088</v>
@@ -23562,7 +23253,7 @@
         <v>714</v>
       </c>
       <c r="B616" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="C616" t="s">
         <v>371</v>
@@ -23591,7 +23282,7 @@
         <v>610</v>
       </c>
       <c r="B617" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="C617" t="s">
         <v>1226</v>
@@ -23620,7 +23311,7 @@
         <v>717</v>
       </c>
       <c r="B618" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="C618" t="s">
         <v>775</v>
@@ -23649,10 +23340,10 @@
         <v>601</v>
       </c>
       <c r="B619" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="C619" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="D619" t="s">
         <v>815</v>
@@ -23678,10 +23369,10 @@
         <v>620</v>
       </c>
       <c r="B620" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="C620" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="D620" t="s">
         <v>815</v>
@@ -23707,10 +23398,10 @@
         <v>606</v>
       </c>
       <c r="B621" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="C621" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="D621" t="s">
         <v>334</v>
@@ -23736,7 +23427,7 @@
         <v>619</v>
       </c>
       <c r="B622" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="C622" t="s">
         <v>658</v>
@@ -23765,10 +23456,10 @@
         <v>726</v>
       </c>
       <c r="B623" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="C623" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="D623" t="s">
         <v>1184</v>
@@ -23794,7 +23485,7 @@
         <v>612</v>
       </c>
       <c r="B624" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
       <c r="C624" t="s">
         <v>1183</v>
@@ -23823,7 +23514,7 @@
         <v>608</v>
       </c>
       <c r="B625" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="C625" t="s">
         <v>1054</v>
@@ -23852,7 +23543,7 @@
         <v>616</v>
       </c>
       <c r="B626" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="C626" t="s">
         <v>1001</v>
@@ -23881,10 +23572,10 @@
         <v>725</v>
       </c>
       <c r="B627" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
       <c r="C627" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
       <c r="D627" t="s">
         <v>881</v>
@@ -23910,10 +23601,10 @@
         <v>613</v>
       </c>
       <c r="B628" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
       <c r="C628" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="D628" t="s">
         <v>1265</v>
@@ -23939,10 +23630,10 @@
         <v>604</v>
       </c>
       <c r="B629" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="C629" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="D629" t="s">
         <v>1271</v>
@@ -23968,10 +23659,10 @@
         <v>609</v>
       </c>
       <c r="B630" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="C630" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="D630" t="s">
         <v>765</v>
@@ -24000,7 +23691,7 @@
         <v>607</v>
       </c>
       <c r="C631" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="D631" t="s">
         <v>14</v>
@@ -24029,7 +23720,7 @@
         <v>757</v>
       </c>
       <c r="C632" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D632" t="s">
         <v>736</v>
@@ -24055,10 +23746,10 @@
         <v>615</v>
       </c>
       <c r="B633" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="C633" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="D633" t="s">
         <v>685</v>
@@ -24084,10 +23775,10 @@
         <v>611</v>
       </c>
       <c r="B634" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="C634" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D634" t="s">
         <v>14</v>
@@ -24113,10 +23804,10 @@
         <v>622</v>
       </c>
       <c r="B635" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="C635" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D635" t="s">
         <v>892</v>
@@ -24142,10 +23833,10 @@
         <v>618</v>
       </c>
       <c r="B636" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="C636" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="D636" t="s">
         <v>969</v>
@@ -24171,10 +23862,10 @@
         <v>722</v>
       </c>
       <c r="B637" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="C637" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D637" t="s">
         <v>1223</v>
@@ -24200,10 +23891,10 @@
         <v>614</v>
       </c>
       <c r="B638" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="C638" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D638" t="s">
         <v>808</v>
@@ -24229,13 +23920,13 @@
         <v>621</v>
       </c>
       <c r="B639" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="C639" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D639" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="E639" t="s">
         <v>750</v>
@@ -24258,7 +23949,7 @@
         <v>627</v>
       </c>
       <c r="B640" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="C640" t="s">
         <v>362</v>
@@ -24287,10 +23978,10 @@
         <v>623</v>
       </c>
       <c r="B641" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="C641" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="D641" t="s">
         <v>848</v>
@@ -24316,7 +24007,7 @@
         <v>629</v>
       </c>
       <c r="B642" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="C642" t="s">
         <v>775</v>
@@ -24345,10 +24036,10 @@
         <v>632</v>
       </c>
       <c r="B643" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="C643" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="D643" t="s">
         <v>334</v>
@@ -24374,10 +24065,10 @@
         <v>625</v>
       </c>
       <c r="B644" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="C644" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="D644" t="s">
         <v>1099</v>
@@ -24403,7 +24094,7 @@
         <v>617</v>
       </c>
       <c r="B645" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="C645" t="s">
         <v>852</v>
@@ -24432,7 +24123,7 @@
         <v>631</v>
       </c>
       <c r="B646" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
       <c r="C646" t="s">
         <v>1111</v>
@@ -24461,7 +24152,7 @@
         <v>624</v>
       </c>
       <c r="B647" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
       <c r="C647" t="s">
         <v>388</v>
@@ -24490,10 +24181,10 @@
         <v>634</v>
       </c>
       <c r="B648" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
       <c r="C648" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="D648" t="s">
         <v>1062</v>
@@ -24519,13 +24210,13 @@
         <v>713</v>
       </c>
       <c r="B649" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="C649" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="D649" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="E649" t="s">
         <v>750</v>
@@ -24548,7 +24239,7 @@
         <v>633</v>
       </c>
       <c r="B650" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="C650" t="s">
         <v>683</v>
@@ -24577,7 +24268,7 @@
         <v>626</v>
       </c>
       <c r="B651" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
       <c r="C651" t="s">
         <v>1021</v>
@@ -24606,13 +24297,13 @@
         <v>630</v>
       </c>
       <c r="B652" t="s">
+        <v>1646</v>
+      </c>
+      <c r="C652" t="s">
+        <v>1647</v>
+      </c>
+      <c r="D652" t="s">
         <v>1648</v>
-      </c>
-      <c r="C652" t="s">
-        <v>1649</v>
-      </c>
-      <c r="D652" t="s">
-        <v>1650</v>
       </c>
       <c r="E652" t="s">
         <v>750</v>
@@ -24635,10 +24326,10 @@
         <v>628</v>
       </c>
       <c r="B653" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="C653" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D653" t="s">
         <v>892</v>
@@ -24664,7 +24355,7 @@
         <v>638</v>
       </c>
       <c r="B654" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="C654" t="s">
         <v>973</v>
@@ -24693,10 +24384,10 @@
         <v>635</v>
       </c>
       <c r="B655" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
       <c r="C655" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="D655" t="s">
         <v>1067</v>
@@ -24722,10 +24413,10 @@
         <v>637</v>
       </c>
       <c r="B656" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="C656" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="D656" t="s">
         <v>690</v>
@@ -24751,10 +24442,10 @@
         <v>641</v>
       </c>
       <c r="B657" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="C657" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="D657" t="s">
         <v>1099</v>
@@ -24780,10 +24471,10 @@
         <v>720</v>
       </c>
       <c r="B658" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="C658" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D658" t="s">
         <v>1184</v>
@@ -24809,7 +24500,7 @@
         <v>636</v>
       </c>
       <c r="B659" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
       <c r="C659" t="s">
         <v>692</v>
@@ -24838,7 +24529,7 @@
         <v>643</v>
       </c>
       <c r="B660" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="C660" t="s">
         <v>852</v>
@@ -24867,7 +24558,7 @@
         <v>640</v>
       </c>
       <c r="B661" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="C661" t="s">
         <v>920</v>
@@ -24925,10 +24616,10 @@
         <v>704</v>
       </c>
       <c r="B663" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="C663" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="D663" t="s">
         <v>803</v>
@@ -24954,10 +24645,10 @@
         <v>708</v>
       </c>
       <c r="B664" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="C664" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="D664" t="s">
         <v>825</v>
@@ -24983,10 +24674,10 @@
         <v>706</v>
       </c>
       <c r="B665" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
       <c r="C665" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D665" t="s">
         <v>315</v>
@@ -25012,10 +24703,10 @@
         <v>705</v>
       </c>
       <c r="B666" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
       <c r="C666" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="D666" t="s">
         <v>382</v>
@@ -25041,10 +24732,10 @@
         <v>642</v>
       </c>
       <c r="B667" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="C667" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
       <c r="D667" t="s">
         <v>306</v>
@@ -25070,10 +24761,10 @@
         <v>644</v>
       </c>
       <c r="B668" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
       <c r="C668" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D668" t="s">
         <v>14</v>
@@ -25099,10 +24790,10 @@
         <v>645</v>
       </c>
       <c r="B669" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="C669" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="D669" t="s">
         <v>812</v>

</xml_diff>